<commit_message>
updated init xlsx file
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v3.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v3.xlsx
@@ -126,9 +126,6 @@
     <t>TrendReportVars_CS3</t>
   </si>
   <si>
-    <t>trend_report_variables_v4.xlsx</t>
-  </si>
-  <si>
     <t>A17</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>I17</t>
   </si>
   <si>
-    <t>E191</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -211,6 +205,12 @@
   </si>
   <si>
     <t>Demands_Deliveries</t>
+  </si>
+  <si>
+    <t>trend_report_variables_v5.xlsx</t>
+  </si>
+  <si>
+    <t>E238</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -610,21 +610,21 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -638,35 +638,35 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,21 +680,21 @@
         <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -745,10 +745,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -769,32 +769,32 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init xlsx file for eflows
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v3.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v3.xlsx
@@ -126,27 +126,9 @@
     <t>TrendReportVars_CS3</t>
   </si>
   <si>
-    <t>A17</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>G17</t>
-  </si>
-  <si>
-    <t>H17</t>
-  </si>
-  <si>
-    <t>I17</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
-    <t>B17</t>
-  </si>
-  <si>
     <t>coeqwal_cs3_scenario_listing_v5.xlsx</t>
   </si>
   <si>
@@ -159,9 +141,6 @@
     <t>SV Dss path names</t>
   </si>
   <si>
-    <t>J17</t>
-  </si>
-  <si>
     <t>cs3rpt2022_all_demand_units_v20250113.xlsx</t>
   </si>
   <si>
@@ -211,6 +190,27 @@
   </si>
   <si>
     <t>E238</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>B18</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>G18</t>
+  </si>
+  <si>
+    <t>H18</t>
+  </si>
+  <si>
+    <t>I18</t>
+  </si>
+  <si>
+    <t>J18</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -610,21 +610,21 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -638,35 +638,35 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,21 +680,21 @@
         <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -745,10 +745,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -769,32 +769,32 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init xlsx file to include S_SLUIS
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v3.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v3.xlsx
@@ -189,9 +189,6 @@
     <t>trend_report_variables_v5.xlsx</t>
   </si>
   <si>
-    <t>E238</t>
-  </si>
-  <si>
     <t>A18</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>J18</t>
+  </si>
+  <si>
+    <t>E239</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +610,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -624,7 +624,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -638,7 +638,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -652,7 +652,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -666,7 +666,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,7 +680,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -694,7 +694,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>